<commit_message>
Linear model - working
</commit_message>
<xml_diff>
--- a/data/main_data.xlsx
+++ b/data/main_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szczy\Desktop\STUDIA\Magisterka sem1\Data_Analytics\Project\Predicting-USA-presidential-elections\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DA61D4-ADAB-4B23-BE88-80E9949B314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6592EE1A-B62B-4623-8826-7429553743AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1350,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J71" sqref="J71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2754,7 +2754,7 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="D70" s="8">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="E70" s="5">
         <v>0.92300000000000004</v>
@@ -2774,7 +2774,7 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="D71" s="8">
-        <v>3</v>
+        <v>0.03</v>
       </c>
       <c r="E71" s="5">
         <v>0.93899999999999995</v>
@@ -2794,7 +2794,7 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="D72" s="8">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="E72" s="5">
         <v>0.94499999999999995</v>
@@ -2814,7 +2814,7 @@
         <v>0.92200000000000004</v>
       </c>
       <c r="D73" s="8">
-        <v>7</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E73" s="5">
         <v>0.94099999999999995</v>

</xml_diff>